<commit_message>
Added monthly keyword data including 'CSR' and created a new line graph
</commit_message>
<xml_diff>
--- a/Sustainability_Interest_Over_Time/Monthly_KW_Data/2014.xlsx
+++ b/Sustainability_Interest_Over_Time/Monthly_KW_Data/2014.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="223">
   <si>
     <t>Published</t>
   </si>
@@ -461,6 +461,54 @@
     <t>http://dnpi.go.id/portal/id/berita/berita-terbaru/304-perubahan-iklim-memperkuat-kapasitas-adaptasi</t>
   </si>
   <si>
+    <t>2014-12-17T20:00:46+07:00</t>
+  </si>
+  <si>
+    <t>CSR</t>
+  </si>
+  <si>
+    <t>Tata Raih Penghargaan CSR dari Dompet Dhuafa | Republika Online</t>
+  </si>
+  <si>
+    <t>http://www.republika.co.id/berita/otomotif/mobil/14/12/17/ngq9h8-tata-raih-penghargaan-csr-dari-dompet-dhuafa</t>
+  </si>
+  <si>
+    <t>2014-12-18T14:05:34+07:00</t>
+  </si>
+  <si>
+    <t>PKS | Ahmad Heryawan Targetkan Pembuatan 500 Ribu Sumur Resapan</t>
+  </si>
+  <si>
+    <t>http://pks.or.id/content/ahmad-heryawan-targetkan-pembuatan-500-ribu-sumur-resapan</t>
+  </si>
+  <si>
+    <t>pks.or.id</t>
+  </si>
+  <si>
+    <t>2014-11-30T11:41:40+07:00</t>
+  </si>
+  <si>
+    <t>Sarihusada Kembali Raih Indonesian CSR Awards 2014 | Republika Online</t>
+  </si>
+  <si>
+    <t>http://www.republika.co.id/berita/nasional/umum/14/11/30/nfu4r0-sarihusada-kembali-raih-indonesian-csr-awards-2014</t>
+  </si>
+  <si>
+    <t>2014-11-21T14:57:52+07:00</t>
+  </si>
+  <si>
+    <t>BRI Ternyata Lahir dari Kas Masjid | Fajar Online</t>
+  </si>
+  <si>
+    <t>http://fajar.co.id/2014/11/21/bri-ternyata-lahir-dari-kas-masjid.html</t>
+  </si>
+  <si>
+    <t>fajar.co.id</t>
+  </si>
+  <si>
+    <t>fajar online</t>
+  </si>
+  <si>
     <t>2014-12-14T11:15:47+07:00</t>
   </si>
   <si>
@@ -582,12 +630,6 @@
   </si>
   <si>
     <t>http://fajar.co.id/2014/12/07/earth-hour-makassar-kumpul-belajar-bareng.html</t>
-  </si>
-  <si>
-    <t>fajar.co.id</t>
-  </si>
-  <si>
-    <t>fajar online</t>
   </si>
   <si>
     <t>2014-06-05T13:29:36+07:00</t>
@@ -683,7 +725,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O56"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2375,10 +2417,10 @@
         <v>152</v>
       </c>
       <c r="E39" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="F39" t="s">
-        <v>154</v>
+        <v>24</v>
       </c>
       <c r="G39" t="n">
         <v>0.0</v>
@@ -2387,42 +2429,42 @@
         <v>0.0</v>
       </c>
       <c r="I39" t="n">
-        <v>529.0</v>
+        <v>25.0</v>
       </c>
       <c r="J39" t="n">
-        <v>41.0</v>
+        <v>1.0</v>
       </c>
       <c r="K39" t="n">
-        <v>21.0</v>
+        <v>0.0</v>
       </c>
       <c r="L39" t="n">
-        <v>16.0</v>
+        <v>1.0</v>
       </c>
       <c r="M39" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="N39" t="n">
-        <v>570.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B40" t="s">
         <v>150</v>
       </c>
       <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E40" t="s">
         <v>156</v>
       </c>
-      <c r="D40" t="s">
-        <v>157</v>
-      </c>
-      <c r="E40" t="s">
-        <v>35</v>
-      </c>
       <c r="F40" t="s">
-        <v>158</v>
+        <v>24</v>
       </c>
       <c r="G40" t="n">
         <v>0.0</v>
@@ -2431,42 +2473,42 @@
         <v>0.0</v>
       </c>
       <c r="I40" t="n">
-        <v>424.0</v>
+        <v>12.0</v>
       </c>
       <c r="J40" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="K40" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L40" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="M40" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="N40" t="n">
-        <v>429.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B41" t="s">
         <v>150</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E41" t="s">
-        <v>162</v>
+        <v>115</v>
       </c>
       <c r="F41" t="s">
-        <v>163</v>
+        <v>24</v>
       </c>
       <c r="G41" t="n">
         <v>0.0</v>
@@ -2475,13 +2517,13 @@
         <v>0.0</v>
       </c>
       <c r="I41" t="n">
-        <v>404.0</v>
+        <v>11.0</v>
       </c>
       <c r="J41" t="n">
-        <v>5.0</v>
+        <v>11.0</v>
       </c>
       <c r="K41" t="n">
-        <v>1.0</v>
+        <v>7.0</v>
       </c>
       <c r="L41" t="n">
         <v>4.0</v>
@@ -2490,27 +2532,27 @@
         <v>0.0</v>
       </c>
       <c r="N41" t="n">
-        <v>409.0</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B42" t="s">
         <v>150</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D42" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
       <c r="F42" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="G42" t="n">
         <v>0.0</v>
@@ -2519,39 +2561,39 @@
         <v>0.0</v>
       </c>
       <c r="I42" t="n">
-        <v>245.0</v>
+        <v>3.0</v>
       </c>
       <c r="J42" t="n">
-        <v>36.0</v>
+        <v>2.0</v>
       </c>
       <c r="K42" t="n">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="L42" t="n">
-        <v>20.0</v>
+        <v>2.0</v>
       </c>
       <c r="M42" t="n">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="N42" t="n">
-        <v>281.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" t="s">
         <v>167</v>
       </c>
-      <c r="B43" t="s">
-        <v>150</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>168</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>169</v>
-      </c>
-      <c r="E43" t="s">
-        <v>57</v>
       </c>
       <c r="F43" t="s">
         <v>170</v>
@@ -2563,22 +2605,22 @@
         <v>0.0</v>
       </c>
       <c r="I43" t="n">
-        <v>235.0</v>
+        <v>529.0</v>
       </c>
       <c r="J43" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="K43" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="L43" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="M43" t="n">
         <v>4.0</v>
       </c>
-      <c r="K43" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="L43" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0.0</v>
-      </c>
       <c r="N43" t="n">
-        <v>239.0</v>
+        <v>570.0</v>
       </c>
     </row>
     <row r="44">
@@ -2586,7 +2628,7 @@
         <v>171</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C44" t="s">
         <v>172</v>
@@ -2595,10 +2637,10 @@
         <v>173</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F44" t="s">
-        <v>24</v>
+        <v>174</v>
       </c>
       <c r="G44" t="n">
         <v>0.0</v>
@@ -2607,42 +2649,42 @@
         <v>0.0</v>
       </c>
       <c r="I44" t="n">
-        <v>145.0</v>
+        <v>424.0</v>
       </c>
       <c r="J44" t="n">
-        <v>20.0</v>
+        <v>5.0</v>
       </c>
       <c r="K44" t="n">
-        <v>7.0</v>
+        <v>1.0</v>
       </c>
       <c r="L44" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="M44" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="N44" t="n">
-        <v>165.0</v>
+        <v>429.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C45" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D45" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E45" t="s">
-        <v>40</v>
+        <v>178</v>
       </c>
       <c r="F45" t="s">
-        <v>24</v>
+        <v>179</v>
       </c>
       <c r="G45" t="n">
         <v>0.0</v>
@@ -2651,39 +2693,39 @@
         <v>0.0</v>
       </c>
       <c r="I45" t="n">
-        <v>140.0</v>
+        <v>404.0</v>
       </c>
       <c r="J45" t="n">
-        <v>9.0</v>
+        <v>5.0</v>
       </c>
       <c r="K45" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="L45" t="n">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="M45" t="n">
         <v>0.0</v>
       </c>
       <c r="N45" t="n">
-        <v>149.0</v>
+        <v>409.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B46" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D46" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E46" t="s">
-        <v>180</v>
+        <v>40</v>
       </c>
       <c r="F46" t="s">
         <v>24</v>
@@ -2695,42 +2737,42 @@
         <v>0.0</v>
       </c>
       <c r="I46" t="n">
-        <v>4.0</v>
+        <v>245.0</v>
       </c>
       <c r="J46" t="n">
-        <v>0.0</v>
+        <v>36.0</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="M46" t="n">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="N46" t="n">
-        <v>4.0</v>
+        <v>281.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B47" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
       <c r="D47" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="E47" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="F47" t="s">
-        <v>24</v>
+        <v>186</v>
       </c>
       <c r="G47" t="n">
         <v>0.0</v>
@@ -2739,36 +2781,36 @@
         <v>0.0</v>
       </c>
       <c r="I47" t="n">
-        <v>2.0</v>
+        <v>235.0</v>
       </c>
       <c r="J47" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="K47" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="L47" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="M47" t="n">
         <v>0.0</v>
       </c>
       <c r="N47" t="n">
-        <v>2.0</v>
+        <v>239.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C48" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="D48" t="s">
-        <v>44</v>
+        <v>189</v>
       </c>
       <c r="E48" t="s">
         <v>40</v>
@@ -2780,86 +2822,86 @@
         <v>0.0</v>
       </c>
       <c r="H48" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I48" t="n">
-        <v>274.0</v>
+        <v>145.0</v>
       </c>
       <c r="J48" t="n">
-        <v>52.0</v>
+        <v>20.0</v>
       </c>
       <c r="K48" t="n">
-        <v>36.0</v>
+        <v>7.0</v>
       </c>
       <c r="L48" t="n">
-        <v>16.0</v>
+        <v>9.0</v>
       </c>
       <c r="M48" t="n">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="N48" t="n">
-        <v>327.0</v>
+        <v>165.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>190</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C49" t="s">
-        <v>66</v>
+        <v>191</v>
       </c>
       <c r="D49" t="s">
-        <v>67</v>
+        <v>192</v>
       </c>
       <c r="E49" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="F49" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="G49" t="n">
         <v>0.0</v>
       </c>
       <c r="H49" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I49" t="n">
-        <v>118.0</v>
+        <v>140.0</v>
       </c>
       <c r="J49" t="n">
-        <v>273.0</v>
+        <v>9.0</v>
       </c>
       <c r="K49" t="n">
-        <v>174.0</v>
+        <v>3.0</v>
       </c>
       <c r="L49" t="n">
-        <v>77.0</v>
+        <v>6.0</v>
       </c>
       <c r="M49" t="n">
-        <v>22.0</v>
+        <v>0.0</v>
       </c>
       <c r="N49" t="n">
-        <v>392.0</v>
+        <v>149.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C50" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D50" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="E50" t="s">
-        <v>40</v>
+        <v>196</v>
       </c>
       <c r="F50" t="s">
         <v>24</v>
@@ -2871,42 +2913,42 @@
         <v>0.0</v>
       </c>
       <c r="I50" t="n">
-        <v>96.0</v>
+        <v>4.0</v>
       </c>
       <c r="J50" t="n">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="K50" t="n">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="L50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N50" t="n">
         <v>4.0</v>
-      </c>
-      <c r="M50" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N50" t="n">
-        <v>105.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
       <c r="B51" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>134</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="E51" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="F51" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G51" t="n">
         <v>0.0</v>
@@ -2915,124 +2957,124 @@
         <v>0.0</v>
       </c>
       <c r="I51" t="n">
-        <v>43.0</v>
+        <v>2.0</v>
       </c>
       <c r="J51" t="n">
-        <v>69.0</v>
+        <v>0.0</v>
       </c>
       <c r="K51" t="n">
-        <v>27.0</v>
+        <v>0.0</v>
       </c>
       <c r="L51" t="n">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="M51" t="n">
-        <v>11.0</v>
+        <v>0.0</v>
       </c>
       <c r="N51" t="n">
-        <v>112.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C52" t="s">
-        <v>188</v>
+        <v>43</v>
       </c>
       <c r="D52" t="s">
-        <v>189</v>
+        <v>44</v>
       </c>
       <c r="E52" t="s">
-        <v>190</v>
+        <v>40</v>
       </c>
       <c r="F52" t="s">
-        <v>191</v>
+        <v>24</v>
       </c>
       <c r="G52" t="n">
         <v>0.0</v>
       </c>
       <c r="H52" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I52" t="n">
-        <v>24.0</v>
+        <v>274.0</v>
       </c>
       <c r="J52" t="n">
-        <v>0.0</v>
+        <v>52.0</v>
       </c>
       <c r="K52" t="n">
-        <v>0.0</v>
+        <v>36.0</v>
       </c>
       <c r="L52" t="n">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c r="M52" t="n">
         <v>0.0</v>
       </c>
       <c r="N52" t="n">
-        <v>24.0</v>
+        <v>327.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>192</v>
+        <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C53" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="D53" t="s">
-        <v>194</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
-        <v>195</v>
+        <v>18</v>
       </c>
       <c r="F53" t="s">
-        <v>196</v>
+        <v>68</v>
       </c>
       <c r="G53" t="n">
         <v>0.0</v>
       </c>
       <c r="H53" t="n">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="I53" t="n">
-        <v>11.0</v>
+        <v>118.0</v>
       </c>
       <c r="J53" t="n">
-        <v>50.0</v>
+        <v>273.0</v>
       </c>
       <c r="K53" t="n">
-        <v>25.0</v>
+        <v>174.0</v>
       </c>
       <c r="L53" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="M53" t="n">
         <v>22.0</v>
       </c>
-      <c r="M53" t="n">
-        <v>3.0</v>
-      </c>
       <c r="N53" t="n">
-        <v>73.0</v>
+        <v>392.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B54" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C54" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D54" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E54" t="s">
         <v>40</v>
@@ -3047,42 +3089,42 @@
         <v>0.0</v>
       </c>
       <c r="I54" t="n">
-        <v>21.0</v>
+        <v>96.0</v>
       </c>
       <c r="J54" t="n">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="K54" t="n">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="L54" t="n">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="M54" t="n">
         <v>0.0</v>
       </c>
       <c r="N54" t="n">
-        <v>23.0</v>
+        <v>105.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>200</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>203</v>
+        <v>18</v>
       </c>
       <c r="F55" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G55" t="n">
         <v>0.0</v>
@@ -3091,65 +3133,241 @@
         <v>0.0</v>
       </c>
       <c r="I55" t="n">
-        <v>19.0</v>
+        <v>43.0</v>
       </c>
       <c r="J55" t="n">
-        <v>0.0</v>
+        <v>69.0</v>
       </c>
       <c r="K55" t="n">
-        <v>0.0</v>
+        <v>27.0</v>
       </c>
       <c r="L55" t="n">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="M55" t="n">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="N55" t="n">
-        <v>19.0</v>
+        <v>112.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>203</v>
+      </c>
+      <c r="B56" t="s">
+        <v>199</v>
+      </c>
+      <c r="C56" t="s">
         <v>204</v>
       </c>
-      <c r="B56" t="s">
-        <v>183</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>205</v>
       </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
+        <v>163</v>
+      </c>
+      <c r="F56" t="s">
+        <v>164</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I56" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N56" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
         <v>206</v>
       </c>
-      <c r="E56" t="s">
+      <c r="B57" t="s">
+        <v>199</v>
+      </c>
+      <c r="C57" t="s">
         <v>207</v>
       </c>
-      <c r="F56" t="s">
+      <c r="D57" t="s">
         <v>208</v>
       </c>
-      <c r="G56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="I56" t="n">
+      <c r="E57" t="s">
+        <v>209</v>
+      </c>
+      <c r="F57" t="s">
+        <v>210</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H57" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="I57" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="J57" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="K57" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="L57" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="M57" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="N57" t="n">
+        <v>73.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>211</v>
+      </c>
+      <c r="B58" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" t="s">
+        <v>212</v>
+      </c>
+      <c r="D58" t="s">
+        <v>213</v>
+      </c>
+      <c r="E58" t="s">
+        <v>40</v>
+      </c>
+      <c r="F58" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="J58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L58" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N58" t="n">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>214</v>
+      </c>
+      <c r="B59" t="s">
+        <v>199</v>
+      </c>
+      <c r="C59" t="s">
+        <v>215</v>
+      </c>
+      <c r="D59" t="s">
+        <v>216</v>
+      </c>
+      <c r="E59" t="s">
+        <v>217</v>
+      </c>
+      <c r="F59" t="s">
+        <v>24</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I59" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N59" t="n">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>218</v>
+      </c>
+      <c r="B60" t="s">
+        <v>199</v>
+      </c>
+      <c r="C60" t="s">
+        <v>219</v>
+      </c>
+      <c r="D60" t="s">
+        <v>220</v>
+      </c>
+      <c r="E60" t="s">
+        <v>221</v>
+      </c>
+      <c r="F60" t="s">
+        <v>222</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="I60" t="n">
         <v>4.0</v>
       </c>
-      <c r="J56" t="n">
+      <c r="J60" t="n">
         <v>1.0</v>
       </c>
-      <c r="K56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="L56" t="n">
+      <c r="K60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L60" t="n">
         <v>1.0</v>
       </c>
-      <c r="M56" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="N56" t="n">
+      <c r="M60" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N60" t="n">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>